<commit_message>
reworking to mental health topic page along with data update
</commit_message>
<xml_diff>
--- a/xlsx/Old/studies.xlsx
+++ b/xlsx/Old/studies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\kclad.ds.kcl.ac.uk\anywhere\UserData\PSStore01\k1780970\Desktop\cmhm_29Apr22\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emckclac-my.sharepoint.com/personal/k1780970_kcl_ac_uk/Documents/1. Catalogue + work documents/1. Catalogue shared files/1. Catalogue/2. Catalogue study updates/Resource folders/cmhm_20May22/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{6F82A259-41A7-4DF6-B3CE-4CB00C898517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EAD59A3-9B75-4387-85F3-0A6037894792}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{6F82A259-41A7-4DF6-B3CE-4CB00C898517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E966E06E-B4EC-46DB-8948-BF3F1E250123}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21000" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study details" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="798">
   <si>
     <t>Code</t>
   </si>
@@ -1033,23 +1033,26 @@
 Cognitive measures,
 Cognitive decline,
 Diet and nutrition,
-Sexuality and gender identity,
+Digital technology and social media,
+Education,
+Ethnicity and race,
 Housing,
-Socioeconomic status and deprivation,
 Language and literacy,
 Loneliness and social isolation,
+Personality,
 Migration and immigration,
 Neighbourhood,
 Personality,
 Physical health assessment,
-Digital technology and social media,
-Victimisation and life events,
 Reproductive health,
-Work and employment,
+Sexuality and gender identity,
 Sleep problems,
 Social care - receipt,
 Social care - provision,
-Social care - need</t>
+Social care - need,
+Socioeconomic status and deprivation,
+Victimisation and life events,
+Work and employment</t>
   </si>
   <si>
     <t>England, National</t>
@@ -1306,20 +1309,23 @@
 Biomarkers,
 Cognitive measures,
 Diet and nutrition,
+Ethnicity and race,
 Housing,
-Socioeconomic status and deprivation,
 Language and literacy,
 Loneliness and social isolation,
 Migration and immigration,
 Neighbourhood,
 Personality,
 Physical health assessment,
-Victimisation and life events,
 Puberty,
 Reproductive health,
-Work and employment,
+Sexuality and gender identity,
+Sleep problems,
 Social care - receipt,
-Social care - need</t>
+Social care - need,
+Socioeconomic status and deprivation,
+Victimisation and life events,
+Work and employment</t>
   </si>
   <si>
     <t>Scotland, National</t>
@@ -1701,14 +1707,15 @@
     <t>Covid-19 data collection,
 Biomarkers,
 Cognitive measures,
-Socioeconomic status and deprivation,
+Diet and nutrition,
+Digital technology and social media,
 Language and literacy,
 Loneliness and social isolation,
 Personality,
-Digital technology and social media,
-Victimisation and life events,
 Puberty,
-Sleep problems</t>
+Sleep problems,
+Socioeconomic status and deprivation,
+Victimisation and life events</t>
   </si>
   <si>
     <t>KCLMilitary</t>
@@ -3628,25 +3635,23 @@
     <t>Nationwide (but control participants mostly recruited from London)</t>
   </si>
   <si>
-    <t xml:space="preserve">Participating parents and their children were recruited from a volunteer database at the Birkbeck Centre for Brain and Cognitive Development. Infants could be enrolled in the study if they either had a first degree relative with ASD, a first degree relative with diagnosed or probable ADHD, or no first-degree relatives with either diagnosis. In phases 1 and 2, the children recruited were only at elevated likelihood (EL) for ASD, whilst in phase 3, children are at EL for ASD, ADHD, or both. Phase 3 is also known as BASIS-STAARS (STudying Autism and ADHD riskS). Some children from phase 2 have also been involved in phase 3.
+    <t xml:space="preserve">Participating parents and their children were recruited from a volunteer database at the Birkbeck Centre for Brain and Cognitive Development. Infants could be enrolled in the study if they either had a first degree relative with ASD, a first degree relative with diagnosed or probable ADHD, or no first-degree relatives with either diagnosis. In phases 1 and 2, the children recruited were only at elevated likelihood (EL) for ASD, whilst in phase 3, children are at EL for ASD, ADHD, or both. Phase 3 is known as BASIS-STAARS (STudying Autism and ADHD riskS). Some families have taken part in more than one phase.  
 &lt;br&gt;&lt;br&gt;
-Infants were identified as being at EL if they had at least one older sibling with a community clinical diagnosis of autism, which was confirmed based on parent report using the Development and Wellbeing Assessment (DAWBA; Goodman et al., 2000), the Social Communication Questionnaire (SCQ; Berument et al., 1999) or parent confirmed community clinical autism diagnosis. Infants were identified as being at typical likelihood (TL) if they had at least one older sibling with typical development and no known autism in first-degree family members (as confirmed through parent interviews regarding family medical history). In phase 3, children were recruited and identified as being at EL for ADHD if they had either an older sibling or a parent with a diagnosis of ADHD, also confirmed through parent interviews regarding family history. 
+Infants were identified as being at EL if they had at least one older sibling with a community clinical diagnosis of autism, which was confirmed based on parent report using the Development and Wellbeing Assessment (DAWBA; Goodman et al., 2000), the Social Communication Questionnaire (SCQ; Berument et al., 1999) or parent confirmed community clinical autism diagnosis. Infants were identified as being at typical likelihood (TL) if they had at least one older sibling with typical development and no known autism in first-degree family members (as confirmed through parent interviews regarding family medical history). In phase 3, children were recruited and identified as being at EL for ADHD if they had either an older sibling or a parent with a diagnosis of ADHD,  confirmed through parent report using the Conner's Parent Rating Scale, and Conner's Adult. 
 &lt;br&gt;&lt;br&gt;
-Cohort members have been assessed at approximately 1, 5, 8, 14, 24, and 36 months, before being followed up during mid-childhood at approximately age 7 to 11 years. The follow up of children at mid-childhood in phase 1 is known as ‘BASIS-7’, whilst follow up for phases 2 and 3 is known as ‘SuperSTAARS’. Participants are administered a range of experimental, behavioural and cognitive tasks and interactive assessments of autistic symptomatology. Parents also complete a range of questionnaires and interviews relating to different aspects of early development. Phase 1 data collection ran from 2006-2015, phase 2 from 2009-2019, and phase 3 from 2013-present. 
+Cohort members have been assessed at approximately 1, 5, 8, 14, 24, and 36 months, before being followed up during mid-childhood at approximately age 7 to 11 years. The follow up of children at mid-childhood in phase 1 is known as ‘BASIS-7’, whilst follow up for phases 2 and 3 is known as ‘SuperSTAARS’. Participants are administered a range of experimental, behavioural and cognitive tasks and interactive assessments of autistic symptomatology. Parents also complete a range of questionnaires and interviews relating to different aspects of early development. Phase 1 data collection ran from 2006-2015, phase 2 from 2009-2022, and phase 3 from 2013-2023. 
 </t>
   </si>
   <si>
     <t xml:space="preserve">Phase 1: 104&lt;br&gt;
 Phase 2: 143&lt;br&gt;
-Phase 3.1:  166&lt;br&gt;	
-Phase 3.2: ongoing&lt;br&gt;
+Phase 3: 300
 </t>
   </si>
   <si>
     <t xml:space="preserve">Phase 1: 76&lt;br&gt;
 Phase 2: 97&lt;br&gt;
-Phase 3.1: ongoing&lt;br&gt;
-Phase 3.2: ongoing&lt;br&gt;
+Phase 3: ongoing
 </t>
   </si>
   <si>
@@ -3669,7 +3674,7 @@
 &lt;a href="https://doi.org/10.1111/jcpp.13563"&gt;https://doi.org/10.1111/jcpp.13563&lt;/a&gt;</t>
   </si>
   <si>
-    <t>MRC SFARI AuSpeaks Autistica EUCom IMI</t>
+    <t>MRC SFARI AuSpeaks Autistica EUCom IMI Horizon</t>
   </si>
   <si>
     <t xml:space="preserve">Biomarkers,
@@ -3678,6 +3683,77 @@
 Parenting and family,
 Sleep problems,
 Socioeconomic status and deprivation </t>
+  </si>
+  <si>
+    <t>CSDD</t>
+  </si>
+  <si>
+    <t>The Cambridge Study in Delinquent Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Cambridge Study in Delinquent Development (CSDD) is a prospective longitudinal cohort study of 411 males living in South London, first assessed in 1961. The original aim of the CSDD was to describe the development of delinquent and criminal behaviour in inner-city males, to investigate to what extent this could be predicted in advance, why juvenile delinquency began, and why it did or did not continue into adulthood. The focus was also on continuity in behavioural development, on the effects of life events on development, and on predicting future behaviour. The study was not set up to test any one particular theory of delinquency but aimed to test many different hypotheses about the causes and correlates of offending. </t>
+  </si>
+  <si>
+    <t>University of Cambridge</t>
+  </si>
+  <si>
+    <t>&lt;a href="http://www.crim.cam.ac.uk/People/professor-david-farrington"&gt;http://www.crim.cam.ac.uk/People/professor-david-farrington&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sample is made up of 411 males born in 1952-1953, who were all living in a working-class area of South London at the time of the first assessment. Most of the sample was chosen by taking all the males who were then aged 8-9 and on the registers of 6 state primary schools within a 1-mile radius of the research offices. 12 individuals from a local special educational needs school were also included in the sample. 
+&lt;br&gt;&lt;br&gt;
+Of the 411 males, 87% were White, and of British origin, 12 were African-Caribbean, 14 had at least 1 parent from Ireland, 12 had parents from Cyprus and the other 16 participants were White, with 1 parent from another Western industrialized country. Based on the father’s occupations at the time of recruitment, 94% of the sample could be described as working-class. The sample was thus overwhelmingly a white, urban, working-class sample of British origin.
+&lt;br&gt;&lt;br&gt; 
+The participants have been interviewed 9 times throughout their lives, from ages 8-48 years. At all time points a high proportion of males have been interviewed, except at ages 21 and 25, due to inadequate funding. At these time points, only a subsample of participants were interviewed. Parents and teachers were also interviewed when the boys were aged 8-15, at the family home or in the boy’s school.  
+&lt;br&gt;&lt;br&gt;
+Criminal records were collected up to age 56, so self-report and official records of offending could be analysed. </t>
+  </si>
+  <si>
+    <t>8-9 years</t>
+  </si>
+  <si>
+    <t>1952-1953</t>
+  </si>
+  <si>
+    <t>Researchers wishing to access data should apply to David Farringdon via email on dpf1@cam.ac.uk.</t>
+  </si>
+  <si>
+    <t>Health data,
+Criminal records</t>
+  </si>
+  <si>
+    <t>Some original documentation for the Cambridge Study of Delinquent Development is no longer available, so some sweeps include less detailed information than other studies on the Catalogue. All mental health measures collected in the study from age 18 onwards are listed at item level. 
+&lt;br&gt;&lt;br&gt;
+Original documentation from data collected from age 8 to 15 years are not available, so datasets were used to the collect information displayed on the Catalogue. At these time points, these variables have been listed, but items, response scales and reporting period are not available. The interviews at these time points (ages 8, 10, 12, 14) were conducted with cohort members' parents and teachers and were mainly concerned with early conduct, behaviour and emotional problems, and personality. Self-reported measures were also collected from parents about their own mental health history. 
+&lt;br&gt;&lt;br&gt;
+Variables from interviews with parents and teachers are also not available for the age 16 sweep. However, documentation from employment interviews conducted with the cohort members are available, and these measures are listed at the item level.</t>
+  </si>
+  <si>
+    <t>Farringdon, D. P., Jolliffe, D., &amp; Coid, J. W. (2021). Cohort profile: The Cambridge Study in Delinquent Development (CSDD). Journal of Developmental and Life-Course Criminology, 7, 278-291. 
+&lt;br&gt;
+&lt;a href="https://doi.org/10.1007/s40865-021-00162-y"&gt;https://doi.org/10.1007/s40865-021-00162-y&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>HOUK DfE DoHSC Rayne SRFound BCTrust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cognitive measures,
+Education,
+Housing,
+Language and literacy,
+Parenting and family,
+Personality,
+Physical health assessment,
+Political and social attitudes,
+Sexuality and gender identity,
+Sleep problems,
+Socioeconomic status and deprivation,
+Victimisation and life events,
+Work and employment
+</t>
+  </si>
+  <si>
+    <t>England, local area</t>
   </si>
 </sst>
 </file>
@@ -4336,11 +4412,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AMJ87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H52" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="R14" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="T14" sqref="T14"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="V1" sqref="V1"/>
     </sheetView>
@@ -4362,7 +4439,7 @@
     <col min="14" max="14" width="56" style="2" customWidth="1"/>
     <col min="15" max="15" width="15.28515625" style="2" customWidth="1"/>
     <col min="16" max="16" width="28" style="2" customWidth="1"/>
-    <col min="17" max="17" width="17.28515625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="23" style="2" customWidth="1"/>
     <col min="18" max="18" width="28.85546875" style="2" customWidth="1"/>
     <col min="19" max="19" width="55.28515625" style="2" customWidth="1"/>
     <col min="20" max="20" width="55.140625" style="2" customWidth="1"/>
@@ -4468,7 +4545,7 @@
       <c r="AH1" s="26"/>
       <c r="AMJ1" s="28"/>
     </row>
-    <row r="2" spans="1:1024" s="11" customFormat="1" ht="195" customHeight="1">
+    <row r="2" spans="1:1024" s="11" customFormat="1" ht="195" hidden="1" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
@@ -4555,7 +4632,7 @@
       <c r="AH2" s="8"/>
       <c r="AMJ2"/>
     </row>
-    <row r="3" spans="1:1024" s="14" customFormat="1" ht="101.1" customHeight="1">
+    <row r="3" spans="1:1024" s="14" customFormat="1" ht="101.1" hidden="1" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>50</v>
       </c>
@@ -4644,7 +4721,7 @@
       <c r="AH3" s="5"/>
       <c r="AMJ3"/>
     </row>
-    <row r="4" spans="1:1024" s="14" customFormat="1" ht="99.95" customHeight="1">
+    <row r="4" spans="1:1024" s="14" customFormat="1" ht="99.95" hidden="1" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>70</v>
       </c>
@@ -4731,7 +4808,7 @@
       <c r="AH4" s="5"/>
       <c r="AMJ4"/>
     </row>
-    <row r="5" spans="1:1024" s="2" customFormat="1" ht="110.1" customHeight="1">
+    <row r="5" spans="1:1024" s="2" customFormat="1" ht="110.1" hidden="1" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>90</v>
       </c>
@@ -4815,7 +4892,7 @@
       <c r="AH5" s="5"/>
       <c r="AMJ5"/>
     </row>
-    <row r="6" spans="1:1024" s="14" customFormat="1" ht="276">
+    <row r="6" spans="1:1024" s="14" customFormat="1" ht="276" hidden="1">
       <c r="A6" s="7" t="s">
         <v>106</v>
       </c>
@@ -4902,7 +4979,7 @@
       <c r="AH6" s="2"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" s="16" customFormat="1" ht="131.1" customHeight="1">
+    <row r="7" spans="1:1024" s="16" customFormat="1" ht="131.1" hidden="1" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>122</v>
       </c>
@@ -4989,7 +5066,7 @@
       <c r="AH7" s="2"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" s="14" customFormat="1" ht="120" customHeight="1">
+    <row r="8" spans="1:1024" s="14" customFormat="1" ht="120" hidden="1" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>139</v>
       </c>
@@ -5076,7 +5153,7 @@
       <c r="AH8" s="2"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" s="14" customFormat="1" ht="123.95" customHeight="1">
+    <row r="9" spans="1:1024" s="14" customFormat="1" ht="123.95" hidden="1" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>152</v>
       </c>
@@ -5163,7 +5240,7 @@
       <c r="AH9" s="5"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" s="14" customFormat="1" ht="96" customHeight="1">
+    <row r="10" spans="1:1024" s="14" customFormat="1" ht="96" hidden="1" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>169</v>
       </c>
@@ -5250,7 +5327,7 @@
       <c r="AH10" s="5"/>
       <c r="AMJ10"/>
     </row>
-    <row r="11" spans="1:1024" s="14" customFormat="1" ht="155.1" customHeight="1">
+    <row r="11" spans="1:1024" s="14" customFormat="1" ht="155.1" hidden="1" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>184</v>
       </c>
@@ -5337,7 +5414,7 @@
       <c r="AH11" s="5"/>
       <c r="AMJ11"/>
     </row>
-    <row r="12" spans="1:1024" s="14" customFormat="1" ht="207.95" customHeight="1">
+    <row r="12" spans="1:1024" s="14" customFormat="1" ht="207.95" hidden="1" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>197</v>
       </c>
@@ -5424,7 +5501,7 @@
       <c r="AH12" s="5"/>
       <c r="AMJ12"/>
     </row>
-    <row r="13" spans="1:1024" s="14" customFormat="1" ht="141.94999999999999" customHeight="1">
+    <row r="13" spans="1:1024" s="14" customFormat="1" ht="141.94999999999999" hidden="1" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>210</v>
       </c>
@@ -5509,7 +5586,7 @@
       <c r="AH13" s="2"/>
       <c r="AMJ13"/>
     </row>
-    <row r="14" spans="1:1024" s="16" customFormat="1" ht="114.95" customHeight="1">
+    <row r="14" spans="1:1024" s="16" customFormat="1" ht="162.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>224</v>
       </c>
@@ -5596,7 +5673,7 @@
       <c r="AH14" s="2"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024" s="2" customFormat="1" ht="129.94999999999999" customHeight="1">
+    <row r="15" spans="1:1024" s="2" customFormat="1" ht="129.94999999999999" hidden="1" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>239</v>
       </c>
@@ -5681,7 +5758,7 @@
       <c r="AH15" s="5"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" s="14" customFormat="1" ht="87" customHeight="1">
+    <row r="16" spans="1:1024" s="14" customFormat="1" ht="87" hidden="1" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>255</v>
       </c>
@@ -5766,7 +5843,7 @@
       <c r="AH16" s="5"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024" s="14" customFormat="1" ht="183.95" customHeight="1">
+    <row r="17" spans="1:1024" s="14" customFormat="1" ht="183.95" hidden="1" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>273</v>
       </c>
@@ -5851,7 +5928,7 @@
       <c r="AH17" s="5"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1:1024" s="14" customFormat="1" ht="140.1" customHeight="1">
+    <row r="18" spans="1:1024" s="14" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>287</v>
       </c>
@@ -5938,7 +6015,7 @@
       <c r="AH18" s="2"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1:1024" s="14" customFormat="1" ht="140.1" customHeight="1">
+    <row r="19" spans="1:1024" s="14" customFormat="1" ht="140.1" hidden="1" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>305</v>
       </c>
@@ -6025,7 +6102,7 @@
       <c r="AH19" s="2"/>
       <c r="AMJ19"/>
     </row>
-    <row r="20" spans="1:1024" s="14" customFormat="1" ht="189.95" customHeight="1">
+    <row r="20" spans="1:1024" s="14" customFormat="1" ht="189.95" hidden="1" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>320</v>
       </c>
@@ -6112,7 +6189,7 @@
       <c r="AH20" s="5"/>
       <c r="AMJ20"/>
     </row>
-    <row r="21" spans="1:1024" s="14" customFormat="1" ht="233.1" customHeight="1">
+    <row r="21" spans="1:1024" s="14" customFormat="1" ht="233.1" hidden="1" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>328</v>
       </c>
@@ -6199,7 +6276,7 @@
       <c r="AH21" s="2"/>
       <c r="AMJ21"/>
     </row>
-    <row r="22" spans="1:1024" s="6" customFormat="1" ht="198.95" customHeight="1">
+    <row r="22" spans="1:1024" s="6" customFormat="1" ht="198.95" hidden="1" customHeight="1">
       <c r="A22" s="18" t="s">
         <v>337</v>
       </c>
@@ -6286,7 +6363,7 @@
       <c r="AH22" s="5"/>
       <c r="AMJ22"/>
     </row>
-    <row r="23" spans="1:1024" s="6" customFormat="1" ht="153" customHeight="1">
+    <row r="23" spans="1:1024" s="6" customFormat="1" ht="153" hidden="1" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>353</v>
       </c>
@@ -6460,7 +6537,7 @@
       <c r="AH24" s="2"/>
       <c r="AMJ24"/>
     </row>
-    <row r="25" spans="1:1024" s="6" customFormat="1" ht="216" customHeight="1">
+    <row r="25" spans="1:1024" s="6" customFormat="1" ht="216" hidden="1" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>382</v>
       </c>
@@ -6547,7 +6624,7 @@
       <c r="AH25" s="5"/>
       <c r="AMJ25"/>
     </row>
-    <row r="26" spans="1:1024" s="6" customFormat="1" ht="228" customHeight="1">
+    <row r="26" spans="1:1024" s="6" customFormat="1" ht="228" hidden="1" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>397</v>
       </c>
@@ -6636,7 +6713,7 @@
       <c r="AH26" s="2"/>
       <c r="AMJ26"/>
     </row>
-    <row r="27" spans="1:1024" s="6" customFormat="1" ht="201.95" customHeight="1">
+    <row r="27" spans="1:1024" s="6" customFormat="1" ht="201.95" hidden="1" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>412</v>
       </c>
@@ -6725,7 +6802,7 @@
       <c r="AH27" s="2"/>
       <c r="AMJ27"/>
     </row>
-    <row r="28" spans="1:1024" s="6" customFormat="1" ht="215.1" customHeight="1">
+    <row r="28" spans="1:1024" s="6" customFormat="1" ht="215.1" hidden="1" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>422</v>
       </c>
@@ -6812,7 +6889,7 @@
       <c r="AH28" s="2"/>
       <c r="AMJ28"/>
     </row>
-    <row r="29" spans="1:1024" s="6" customFormat="1" ht="221.1" customHeight="1">
+    <row r="29" spans="1:1024" s="6" customFormat="1" ht="221.1" hidden="1" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>435</v>
       </c>
@@ -6903,7 +6980,7 @@
       <c r="AH29" s="12"/>
       <c r="AMJ29"/>
     </row>
-    <row r="30" spans="1:1024" s="2" customFormat="1" ht="140.1" customHeight="1">
+    <row r="30" spans="1:1024" s="2" customFormat="1" ht="140.1" hidden="1" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>448</v>
       </c>
@@ -6985,7 +7062,7 @@
       <c r="AH30" s="5"/>
       <c r="AMJ30"/>
     </row>
-    <row r="31" spans="1:1024" s="6" customFormat="1" ht="152.1" customHeight="1">
+    <row r="31" spans="1:1024" s="6" customFormat="1" ht="152.1" hidden="1" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>463</v>
       </c>
@@ -7070,7 +7147,7 @@
       <c r="AH31" s="8"/>
       <c r="AMJ31"/>
     </row>
-    <row r="32" spans="1:1024" s="2" customFormat="1" ht="294" customHeight="1">
+    <row r="32" spans="1:1024" s="2" customFormat="1" ht="294" hidden="1" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>477</v>
       </c>
@@ -7156,7 +7233,7 @@
       <c r="AH32" s="5"/>
       <c r="AMJ32"/>
     </row>
-    <row r="33" spans="1:1024" s="6" customFormat="1" ht="264">
+    <row r="33" spans="1:1024" s="6" customFormat="1" ht="264" hidden="1">
       <c r="A33" s="7" t="s">
         <v>490</v>
       </c>
@@ -7243,7 +7320,7 @@
       <c r="AH33" s="2"/>
       <c r="AMJ33"/>
     </row>
-    <row r="34" spans="1:1024" s="6" customFormat="1" ht="228">
+    <row r="34" spans="1:1024" s="6" customFormat="1" ht="228" hidden="1">
       <c r="A34" s="18" t="s">
         <v>502</v>
       </c>
@@ -7332,7 +7409,7 @@
       <c r="AH34" s="5"/>
       <c r="AMJ34"/>
     </row>
-    <row r="35" spans="1:1024" s="6" customFormat="1" ht="288">
+    <row r="35" spans="1:1024" s="6" customFormat="1" ht="288" hidden="1">
       <c r="A35" s="18" t="s">
         <v>519</v>
       </c>
@@ -7421,7 +7498,7 @@
       <c r="AH35" s="5"/>
       <c r="AMJ35"/>
     </row>
-    <row r="36" spans="1:1024" ht="192">
+    <row r="36" spans="1:1024" ht="192" hidden="1">
       <c r="A36" s="7" t="s">
         <v>531</v>
       </c>
@@ -7498,7 +7575,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="37" spans="1:1024" ht="204">
+    <row r="37" spans="1:1024" ht="204" hidden="1">
       <c r="A37" s="7" t="s">
         <v>543</v>
       </c>
@@ -7582,7 +7659,7 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
     </row>
-    <row r="38" spans="1:1024" ht="192">
+    <row r="38" spans="1:1024" ht="192" hidden="1">
       <c r="A38" s="18" t="s">
         <v>558</v>
       </c>
@@ -7657,7 +7734,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="39" spans="1:1024" ht="384">
+    <row r="39" spans="1:1024" ht="384" hidden="1">
       <c r="A39" s="7" t="s">
         <v>572</v>
       </c>
@@ -7734,7 +7811,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="40" spans="1:1024" ht="168">
+    <row r="40" spans="1:1024" ht="168" hidden="1">
       <c r="A40" s="7" t="s">
         <v>587</v>
       </c>
@@ -7818,7 +7895,7 @@
       <c r="AG40" s="2"/>
       <c r="AH40" s="2"/>
     </row>
-    <row r="41" spans="1:1024" ht="300">
+    <row r="41" spans="1:1024" ht="300" hidden="1">
       <c r="A41" s="18" t="s">
         <v>600</v>
       </c>
@@ -7893,7 +7970,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="1:1024" ht="276">
+    <row r="42" spans="1:1024" ht="276" hidden="1">
       <c r="A42" s="18" t="s">
         <v>614</v>
       </c>
@@ -7968,7 +8045,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="43" spans="1:1024" ht="252">
+    <row r="43" spans="1:1024" ht="252" hidden="1">
       <c r="A43" s="18" t="s">
         <v>627</v>
       </c>
@@ -8046,7 +8123,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="44" spans="1:1024" ht="153" customHeight="1">
+    <row r="44" spans="1:1024" ht="153" hidden="1" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>643</v>
       </c>
@@ -8133,7 +8210,7 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
     </row>
-    <row r="45" spans="1:1024" ht="360">
+    <row r="45" spans="1:1024" ht="360" hidden="1">
       <c r="A45" s="18" t="s">
         <v>661</v>
       </c>
@@ -8207,7 +8284,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="46" spans="1:1024" ht="228">
+    <row r="46" spans="1:1024" ht="228" hidden="1">
       <c r="A46" s="7" t="s">
         <v>675</v>
       </c>
@@ -8287,7 +8364,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:1024" ht="300">
+    <row r="47" spans="1:1024" ht="300" hidden="1">
       <c r="A47" s="7" t="s">
         <v>691</v>
       </c>
@@ -8361,7 +8438,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:1024" ht="168">
+    <row r="48" spans="1:1024" ht="168" hidden="1">
       <c r="A48" s="7" t="s">
         <v>705</v>
       </c>
@@ -8435,7 +8512,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="144">
+    <row r="49" spans="1:26" ht="144" hidden="1">
       <c r="A49" s="7" t="s">
         <v>719</v>
       </c>
@@ -8512,7 +8589,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="384.75">
+    <row r="50" spans="1:26" ht="31.5" hidden="1" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>730</v>
       </c>
@@ -8586,7 +8663,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="1:26" ht="300">
+    <row r="51" spans="1:26" ht="25.5" hidden="1" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>741</v>
       </c>
@@ -8660,7 +8737,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="155.1" customHeight="1">
+    <row r="52" spans="1:26" ht="19.5" hidden="1" customHeight="1">
       <c r="A52" s="7" t="s">
         <v>753</v>
       </c>
@@ -8734,7 +8811,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="409.6">
+    <row r="53" spans="1:26" ht="146.25" hidden="1" customHeight="1">
       <c r="A53" s="7" t="s">
         <v>768</v>
       </c>
@@ -8808,8 +8885,82 @@
         <v>183</v>
       </c>
     </row>
-    <row r="54" spans="1:26">
-      <c r="A54" s="7"/>
+    <row r="54" spans="1:26" ht="33.75" hidden="1" customHeight="1">
+      <c r="A54" s="7" t="s">
+        <v>783</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>784</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>785</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="H54" s="2">
+        <v>1961</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="K54" s="2">
+        <v>411</v>
+      </c>
+      <c r="L54" s="2">
+        <v>365</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="N54" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="P54" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="Q54" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="R54" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="S54" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="T54" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="U54" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>796</v>
+      </c>
+      <c r="W54" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>797</v>
+      </c>
+      <c r="Z54" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="55" spans="1:26">
       <c r="A55" s="7"/>
@@ -8911,7 +9062,14 @@
       <c r="A87" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AH53" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:AH54" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ELSA"/>
+        <filter val="GSSFHS"/>
+        <filter val="IMAGEN"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH47">
       <sortCondition ref="A1:A47"/>
     </sortState>

</xml_diff>